<commit_message>
Completat Excel cu CFG, CC si drumurile in graf
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4B55CD-A3A0-4123-85B0-87D451E971C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -12,12 +13,23 @@
     <sheet name="F02.TCs" sheetId="11" r:id="rId3"/>
     <sheet name="WBT-TCs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="124">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -70,12 +82,6 @@
     <t>Path</t>
   </si>
   <si>
-    <t>1 - 2(F) - …</t>
-  </si>
-  <si>
-    <t>1 - 2(T) - …</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
@@ -122,15 +128,6 @@
   </si>
   <si>
     <t>Req02_L03</t>
-  </si>
-  <si>
-    <t>&lt;Req02 CFG &gt;</t>
-  </si>
-  <si>
-    <t>1. Evidenţa filmelor din colecţia personală</t>
-  </si>
-  <si>
-    <t>Un cinefil doreşte să îşi dezvolte un program pentru gestionarea filmelor din colecţia personală. Programul va permite următoarele operaţii:</t>
   </si>
   <si>
     <t>Proiectaţi şi implementaţi o aplicaţie Java pentru rezolvarea problemei propuse. Se va evidenţia o arhitectură stratificată.</t>
@@ -199,49 +196,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>F02.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> cautarea filmelor care au un anumit regizor (sau parti din numele regizorului);</t>
-    </r>
-  </si>
-  <si>
     <t>F02</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">F02. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>cautarea filmelor care au un anumit regizor (sau parti din numele regizorului).</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">F02. Covered source code </t>
@@ -552,12 +507,78 @@
   <si>
     <t>F02_TC07</t>
   </si>
+  <si>
+    <t>Aplicația gestionează piesele componente și produsele finite ale unei companii de producție. Informațiile sunt preluate dintr-un fișier text. Funcționalitățile aplicației sunt:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>F02b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Căutarea unui produs după nume</t>
+    </r>
+  </si>
+  <si>
+    <t>Bodea Denisa</t>
+  </si>
+  <si>
+    <t>Răchită Adrian-Iosif</t>
+  </si>
+  <si>
+    <t>Mihiș Alin-Grig</t>
+  </si>
+  <si>
+    <t>Project 02_inventory</t>
+  </si>
+  <si>
+    <t>F02. Căutarea unui produs, după nume.</t>
+  </si>
+  <si>
+    <t>45(T) -&gt; 46 -&gt; 57</t>
+  </si>
+  <si>
+    <t>45(F) -&gt; 47 -&gt; 48(F) -&gt; 53(F) -&gt; 56 -&gt; 57</t>
+  </si>
+  <si>
+    <t>45(F) -&gt; 47 -&gt; 48(F) -&gt; 53(T) -&gt; 54 -&gt; 57</t>
+  </si>
+  <si>
+    <t>45(F) -&gt; 47 -&gt; 48(T) -&gt; 49(T) -&gt; 50 -&gt; 57</t>
+  </si>
+  <si>
+    <t>45(F) -&gt; 47 -&gt; 48(T) -&gt; 49(F) -&gt; 51 -&gt; 48(T) -&gt; … -&gt; 48(T) -&gt; 49 (T) -&gt; 50 -&gt; 57</t>
+  </si>
+  <si>
+    <t>45(F) -&gt; 47 -&gt; 48(T) -&gt; 49(F) -&gt; 51 -&gt; 48(T) -&gt; … -&gt; 48(F) -&gt; 53 (T) -&gt; 54 -&gt; 57</t>
+  </si>
+  <si>
+    <t>45(F) -&gt; 47 -&gt; 48(T) -&gt; 49(F) -&gt; 51 -&gt; 48(T) -&gt; … -&gt; 48(F) -&gt; 53 (F) -&gt; 56 -&gt; 57</t>
+  </si>
+  <si>
+    <t>4 + 1 = 5</t>
+  </si>
+  <si>
+    <t>16 - 13 + 2 = 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -691,6 +712,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -766,7 +794,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -948,55 +976,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1240,7 +1219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1300,9 +1279,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1315,136 +1332,109 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1453,146 +1443,117 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1604,6 +1565,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1612,23 +1576,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>621030</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>575733</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>194310</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>545517</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6188" name="Picture 4">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002C180000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{545B76B9-7EA6-4F90-95EA-2090F97E0226}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1637,7 +1601,51 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="575733" y="1151467"/>
+          <a:ext cx="4313184" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>284020</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3695</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>88740</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>51723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E22CB4F-9098-557C-2D88-D46288723533}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1645,75 +1653,12 @@
           </a:extLst>
         </a:blip>
         <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5208270" y="1588770"/>
-          <a:ext cx="4724400" cy="4168140"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>440266</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>160867</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>451407</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="440266" y="1278467"/>
-          <a:ext cx="4354541" cy="1354666"/>
+          <a:off x="5237020" y="1624677"/>
+          <a:ext cx="4071920" cy="3830319"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1726,9 +1671,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1766,7 +1711,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1838,7 +1783,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2011,14 +1956,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2026,36 +1971,36 @@
     <col min="15" max="15" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="2:16" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B2" s="31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="D1" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N5" s="27" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
@@ -2066,72 +2011,84 @@
       </c>
       <c r="N6" s="19"/>
       <c r="O6" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="14.55" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="N7" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-    </row>
-    <row r="8" spans="2:16" ht="14.55" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="O7" s="118" t="s">
+        <v>110</v>
+      </c>
+      <c r="P7" s="118">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="N8" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
+        <v>57</v>
+      </c>
+      <c r="O8" s="118" t="s">
+        <v>111</v>
+      </c>
+      <c r="P8" s="118">
+        <v>236</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="N9" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
+        <v>58</v>
+      </c>
+      <c r="O9" s="118" t="s">
+        <v>112</v>
+      </c>
+      <c r="P9" s="118">
+        <v>231</v>
+      </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>37</v>
+      <c r="B10" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:16" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B11" s="29" t="s">
-        <v>48</v>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="117" t="s">
+        <v>109</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:16" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="19" spans="2:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -2144,377 +2101,393 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="20" max="20" width="56.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-    </row>
-    <row r="3" spans="2:20" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B3" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="40"/>
-    </row>
-    <row r="6" spans="2:20" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B6" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
+      <c r="D1" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="119" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="49"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
-      <c r="I6" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="Q6" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
+      <c r="I6" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="Q6" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
       <c r="I8" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q8" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q8" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="26" t="s">
-        <v>1</v>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="26">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
+        <v>30</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="I9" s="30"/>
-      <c r="Q9" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
+      <c r="I9" s="29"/>
+      <c r="Q9" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
       <c r="T9" s="26" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
+        <v>31</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
-      <c r="I10" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="43"/>
-      <c r="Q10" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="R10" s="37" t="s">
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+      <c r="O10" s="120"/>
+      <c r="Q10" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="37"/>
+      <c r="S10" s="51"/>
       <c r="T10" s="26" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
+        <v>32</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="46"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+      <c r="O11" s="120"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="C12" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="46"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+      <c r="O12" s="120"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="C13" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="46"/>
-      <c r="Q13" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="R13" s="33"/>
-      <c r="S13" s="33"/>
-      <c r="T13" s="33"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+      <c r="O13" s="120"/>
+      <c r="Q13" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="46"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I15" s="44"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="46"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="120"/>
       <c r="Q15" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="50" t="s">
+      <c r="R15" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
+      <c r="S15" s="52"/>
+      <c r="T15" s="52"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I16" s="44"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="46"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="120"/>
       <c r="Q16" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="R16" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
+        <v>50</v>
+      </c>
+      <c r="R16" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I17" s="44"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="46"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+      <c r="O17" s="120"/>
       <c r="Q17" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="R17" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
+        <v>51</v>
+      </c>
+      <c r="R17" s="121" t="s">
+        <v>116</v>
+      </c>
+      <c r="S17" s="121"/>
+      <c r="T17" s="121"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I18" s="44"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="46"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="120"/>
+      <c r="O18" s="120"/>
       <c r="Q18" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="R18" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
+        <v>52</v>
+      </c>
+      <c r="R18" s="121" t="s">
+        <v>117</v>
+      </c>
+      <c r="S18" s="121"/>
+      <c r="T18" s="121"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I19" s="44"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="46"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="120"/>
+      <c r="M19" s="120"/>
+      <c r="N19" s="120"/>
+      <c r="O19" s="120"/>
       <c r="Q19" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="R19" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
+        <v>84</v>
+      </c>
+      <c r="R19" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I20" s="44"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="46"/>
+      <c r="I20" s="120"/>
+      <c r="J20" s="120"/>
+      <c r="K20" s="120"/>
+      <c r="L20" s="120"/>
+      <c r="M20" s="120"/>
+      <c r="N20" s="120"/>
+      <c r="O20" s="120"/>
       <c r="Q20" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="R20" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
+        <v>85</v>
+      </c>
+      <c r="R20" s="122" t="s">
+        <v>119</v>
+      </c>
+      <c r="S20" s="122"/>
+      <c r="T20" s="122"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I21" s="44"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="46"/>
+      <c r="I21" s="120"/>
+      <c r="J21" s="120"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="120"/>
+      <c r="M21" s="120"/>
+      <c r="N21" s="120"/>
+      <c r="O21" s="120"/>
       <c r="Q21" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="R21" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
+        <v>86</v>
+      </c>
+      <c r="R21" s="122" t="s">
+        <v>120</v>
+      </c>
+      <c r="S21" s="122"/>
+      <c r="T21" s="122"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I22" s="44"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="46"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="120"/>
+      <c r="N22" s="120"/>
+      <c r="O22" s="120"/>
+      <c r="Q22" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="R22" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I23" s="44"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="46"/>
+      <c r="I23" s="120"/>
+      <c r="J23" s="120"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="120"/>
+      <c r="M23" s="120"/>
+      <c r="N23" s="120"/>
+      <c r="O23" s="120"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I24" s="47"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="49"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="120"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2531,14 +2504,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2547,7 +2512,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -2584,619 +2549,562 @@
   <sheetData>
     <row r="1" spans="2:27" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
+      <c r="D1" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="3" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="12"/>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="70"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B6" s="31"/>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73"/>
+      <c r="R7" s="73"/>
+      <c r="S7" s="73"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="73"/>
+      <c r="V7" s="73"/>
+      <c r="W7" s="73"/>
+      <c r="X7" s="73"/>
+      <c r="Y7" s="73"/>
+      <c r="Z7" s="73"/>
+      <c r="AA7" s="74"/>
+    </row>
+    <row r="8" spans="2:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="71"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" s="66"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="66"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="V8" s="76"/>
+      <c r="W8" s="76"/>
+      <c r="X8" s="76"/>
+      <c r="Y8" s="76"/>
+      <c r="Z8" s="76"/>
+      <c r="AA8" s="77"/>
+    </row>
+    <row r="9" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="71"/>
+      <c r="C9" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="60"/>
+      <c r="F9" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="64"/>
+      <c r="H9" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="64"/>
+      <c r="J9" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="64"/>
+      <c r="L9" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="129"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="93"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="93"/>
-      <c r="R4" s="93"/>
-      <c r="S4" s="93"/>
-      <c r="T4" s="93"/>
-      <c r="U4" s="93"/>
-      <c r="V4" s="93"/>
-      <c r="W4" s="93"/>
-      <c r="X4" s="93"/>
-      <c r="Y4" s="93"/>
-      <c r="Z4" s="93"/>
-      <c r="AA4" s="93"/>
-    </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B6" s="96"/>
-      <c r="C6" s="94" t="s">
+      <c r="M9" s="64"/>
+      <c r="N9" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
-      <c r="P6" s="93"/>
-      <c r="Q6" s="93"/>
-      <c r="R6" s="93"/>
-      <c r="S6" s="93"/>
-      <c r="T6" s="93"/>
-      <c r="U6" s="93"/>
-      <c r="V6" s="93"/>
-      <c r="W6" s="93"/>
-      <c r="X6" s="93"/>
-      <c r="Y6" s="93"/>
-      <c r="Z6" s="93"/>
-      <c r="AA6" s="93"/>
-    </row>
-    <row r="7" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="125" t="s">
+      <c r="R9" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="S9" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="T9" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="53">
+        <v>0</v>
+      </c>
+      <c r="V9" s="53">
+        <v>1</v>
+      </c>
+      <c r="W9" s="53">
+        <v>2</v>
+      </c>
+      <c r="X9" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="126"/>
-      <c r="Q7" s="126"/>
-      <c r="R7" s="126"/>
-      <c r="S7" s="126"/>
-      <c r="T7" s="126"/>
-      <c r="U7" s="126"/>
-      <c r="V7" s="126"/>
-      <c r="W7" s="126"/>
-      <c r="X7" s="126"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="126"/>
-      <c r="AA7" s="127"/>
-    </row>
-    <row r="8" spans="2:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="128"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="122" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="109" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="121"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="121"/>
-      <c r="L8" s="121"/>
-      <c r="M8" s="110"/>
-      <c r="N8" s="118" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" s="119"/>
-      <c r="P8" s="119"/>
-      <c r="Q8" s="119"/>
-      <c r="R8" s="119"/>
-      <c r="S8" s="119"/>
-      <c r="T8" s="120"/>
-      <c r="U8" s="115" t="s">
+      <c r="Y9" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="116"/>
-      <c r="W8" s="116"/>
-      <c r="X8" s="116"/>
-      <c r="Y8" s="116"/>
-      <c r="Z8" s="116"/>
-      <c r="AA8" s="117"/>
-    </row>
-    <row r="9" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="128"/>
-      <c r="C9" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="123"/>
-      <c r="F9" s="109" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="110"/>
-      <c r="H9" s="109" t="s">
+      <c r="Z9" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA9" s="53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
+    </row>
+    <row r="11" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="110"/>
-      <c r="J9" s="109" t="s">
+      <c r="D11" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="K9" s="110"/>
-      <c r="L9" s="109" t="s">
+      <c r="E11" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="M9" s="110"/>
-      <c r="N9" s="113" t="s">
-        <v>57</v>
-      </c>
-      <c r="O9" s="113" t="s">
-        <v>58</v>
-      </c>
-      <c r="P9" s="113" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q9" s="113" t="s">
-        <v>91</v>
-      </c>
-      <c r="R9" s="113" t="s">
+      <c r="F11" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="V11" s="38"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
+    </row>
+    <row r="12" spans="2:27" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="S9" s="113" t="s">
+      <c r="D12" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="T9" s="113" t="s">
+      <c r="E12" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="U9" s="111">
-        <v>0</v>
-      </c>
-      <c r="V9" s="111">
-        <v>1</v>
-      </c>
-      <c r="W9" s="111">
-        <v>2</v>
-      </c>
-      <c r="X9" s="111" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y9" s="111" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z9" s="111" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA9" s="111" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="97" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="97" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="97" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="97" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="114"/>
-      <c r="O10" s="114"/>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="114"/>
-      <c r="R10" s="114"/>
-      <c r="S10" s="114"/>
-      <c r="T10" s="114"/>
-      <c r="U10" s="112"/>
-      <c r="V10" s="112"/>
-      <c r="W10" s="112"/>
-      <c r="X10" s="112"/>
-      <c r="Y10" s="112"/>
-      <c r="Z10" s="112"/>
-      <c r="AA10" s="112"/>
-    </row>
-    <row r="11" spans="2:27" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="98" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="101" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="V12" s="38"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="38"/>
+    </row>
+    <row r="13" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="101" t="s">
+      <c r="C13" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="102" t="s">
+      <c r="D13" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="99" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
+    </row>
+    <row r="14" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="100" t="s">
-        <v>98</v>
-      </c>
-      <c r="O11" s="100"/>
-      <c r="P11" s="100"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="100"/>
-      <c r="S11" s="100"/>
-      <c r="T11" s="100"/>
-      <c r="U11" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="V11" s="103"/>
-      <c r="W11" s="103"/>
-      <c r="X11" s="103"/>
-      <c r="Y11" s="103"/>
-      <c r="Z11" s="103"/>
-      <c r="AA11" s="103"/>
-    </row>
-    <row r="12" spans="2:27" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="101" t="s">
+      <c r="C14" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="E14" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="102" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="M14" s="41"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="43"/>
+      <c r="AA14" s="43"/>
+    </row>
+    <row r="15" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" s="99"/>
-      <c r="J12" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="99"/>
-      <c r="N12" s="100"/>
-      <c r="O12" s="100"/>
-      <c r="P12" s="100"/>
-      <c r="Q12" s="100" t="s">
-        <v>98</v>
-      </c>
-      <c r="R12" s="100"/>
-      <c r="S12" s="100"/>
-      <c r="T12" s="100"/>
-      <c r="U12" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="V12" s="103"/>
-      <c r="W12" s="103"/>
-      <c r="X12" s="103"/>
-      <c r="Y12" s="103"/>
-      <c r="Z12" s="103"/>
-      <c r="AA12" s="103"/>
-    </row>
-    <row r="13" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="98" t="s">
+      <c r="C15" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="D15" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="101" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="102" t="s">
+      <c r="F15" s="41"/>
+      <c r="G15" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="M15" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="43"/>
+      <c r="Y15" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z15" s="43"/>
+      <c r="AA15" s="43"/>
+    </row>
+    <row r="16" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="106"/>
-      <c r="G13" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="J13" s="106"/>
-      <c r="K13" s="106"/>
-      <c r="L13" s="106"/>
-      <c r="M13" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="N13" s="107"/>
-      <c r="O13" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="P13" s="107"/>
-      <c r="Q13" s="107"/>
-      <c r="R13" s="107"/>
-      <c r="S13" s="107"/>
-      <c r="T13" s="107"/>
-      <c r="U13" s="108" t="s">
-        <v>98</v>
-      </c>
-      <c r="V13" s="108"/>
-      <c r="W13" s="108"/>
-      <c r="X13" s="108"/>
-      <c r="Y13" s="108"/>
-      <c r="Z13" s="108"/>
-      <c r="AA13" s="108"/>
-    </row>
-    <row r="14" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="98" t="s">
+      <c r="C16" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="D16" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="M16" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="T16" s="42"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="43"/>
+      <c r="X16" s="43"/>
+      <c r="Y16" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z16" s="43"/>
+      <c r="AA16" s="43"/>
+    </row>
+    <row r="17" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="104" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="102" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="106"/>
-      <c r="I14" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="106"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="M14" s="106"/>
-      <c r="N14" s="107"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
-      <c r="U14" s="108" t="s">
-        <v>98</v>
-      </c>
-      <c r="V14" s="108"/>
-      <c r="W14" s="108"/>
-      <c r="X14" s="108"/>
-      <c r="Y14" s="108"/>
-      <c r="Z14" s="108"/>
-      <c r="AA14" s="108"/>
-    </row>
-    <row r="15" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="98" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="104" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" s="105" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="L15" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="M15" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="N15" s="107"/>
-      <c r="O15" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="U15" s="108"/>
-      <c r="V15" s="108"/>
-      <c r="W15" s="108"/>
-      <c r="X15" s="108"/>
-      <c r="Y15" s="108" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z15" s="108"/>
-      <c r="AA15" s="108"/>
-    </row>
-    <row r="16" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="104" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="104" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="105" t="s">
-        <v>113</v>
-      </c>
-      <c r="F16" s="106"/>
-      <c r="G16" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="106"/>
-      <c r="K16" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="L16" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="M16" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="N16" s="107"/>
-      <c r="O16" s="107"/>
-      <c r="P16" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="T16" s="107"/>
-      <c r="U16" s="108"/>
-      <c r="V16" s="108"/>
-      <c r="W16" s="108"/>
-      <c r="X16" s="108"/>
-      <c r="Y16" s="108" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z16" s="108"/>
-      <c r="AA16" s="108"/>
-    </row>
-    <row r="17" spans="2:27" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="98" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="104" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" s="104" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="105" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="L17" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="M17" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="N17" s="107"/>
-      <c r="O17" s="107"/>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="R17" s="107" t="s">
-        <v>98</v>
-      </c>
-      <c r="S17" s="107"/>
-      <c r="T17" s="107"/>
-      <c r="U17" s="108"/>
-      <c r="V17" s="108"/>
-      <c r="W17" s="108"/>
-      <c r="X17" s="108"/>
-      <c r="Y17" s="108" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z17" s="108"/>
-      <c r="AA17" s="108"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="R17" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="43"/>
+      <c r="Y17" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z17" s="43"/>
+      <c r="AA17" s="43"/>
     </row>
     <row r="21" spans="2:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:M8"/>
-    <mergeCell ref="N8:T8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="D1:G1"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C8"/>
@@ -3213,7 +3121,19 @@
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="U8:AA8"/>
     <mergeCell ref="U9:U10"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:M8"/>
+    <mergeCell ref="N8:T8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="S9:S10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3221,7 +3141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -3246,57 +3166,57 @@
     <col min="15" max="15" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="11"/>
-      <c r="D1" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="3" spans="2:14" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B3" s="77" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
+      <c r="D1" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="88" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="80" t="s">
+      <c r="D4" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="80" t="s">
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="81"/>
+      <c r="L4" s="84"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="79"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="89"/>
+      <c r="B5" s="82"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="93"/>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
@@ -3309,10 +3229,10 @@
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="83"/>
+      <c r="I5" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="86"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3324,11 +3244,11 @@
       <c r="B6" s="13">
         <v>9</v>
       </c>
-      <c r="C6" s="84" t="s">
-        <v>49</v>
+      <c r="C6" s="87" t="s">
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>1</v>
@@ -3342,10 +3262,10 @@
       <c r="H6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="90" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="91"/>
+      <c r="I6" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="95"/>
       <c r="K6" s="14" t="s">
         <v>1</v>
       </c>
@@ -3357,9 +3277,9 @@
       <c r="B7" s="13">
         <v>10</v>
       </c>
-      <c r="C7" s="84"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E7" s="13">
         <v>5</v>
@@ -3373,10 +3293,10 @@
       <c r="H7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="81"/>
+      <c r="I7" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="84"/>
       <c r="K7" s="13" t="s">
         <v>1</v>
       </c>
@@ -3388,7 +3308,7 @@
       <c r="B8" s="13">
         <v>11</v>
       </c>
-      <c r="C8" s="84"/>
+      <c r="C8" s="87"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -3404,10 +3324,10 @@
       <c r="H8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="81"/>
+      <c r="I8" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="84"/>
       <c r="K8" s="13" t="s">
         <v>1</v>
       </c>
@@ -3419,7 +3339,7 @@
       <c r="B9" s="13">
         <v>12</v>
       </c>
-      <c r="C9" s="84"/>
+      <c r="C9" s="87"/>
       <c r="D9" s="10" t="s">
         <v>1</v>
       </c>
@@ -3435,10 +3355,10 @@
       <c r="H9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="81"/>
+      <c r="I9" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="84"/>
       <c r="K9" s="13" t="s">
         <v>1</v>
       </c>
@@ -3450,7 +3370,7 @@
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="85"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="9" t="s">
         <v>1</v>
       </c>
@@ -3466,10 +3386,10 @@
       <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="83"/>
+      <c r="I10" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="86"/>
       <c r="K10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3477,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -3490,92 +3410,92 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="15"/>
     </row>
-    <row r="13" spans="2:14" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="53" t="s">
+    <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="99"/>
+      <c r="H13" s="96" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="N13" s="79"/>
+    </row>
+    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="108" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="104" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="104" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="110" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55" t="s">
+      <c r="I14" s="104" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="104" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="106" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="53" t="s">
+      <c r="M14" s="116" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="75" t="s">
+      <c r="N14" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="N13" s="76"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="L14" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="M14" s="74" t="s">
-        <v>78</v>
-      </c>
-      <c r="N14" s="58" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="67"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="59"/>
-    </row>
-    <row r="16" spans="2:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B15" s="109"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="103"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="107"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="108"/>
+      <c r="N15" s="101"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="19">
         <f>SUM(C16:D16)</f>
         <v>0</v>
@@ -3589,10 +3509,10 @@
       <c r="E16" s="17"/>
       <c r="F16" s="18"/>
       <c r="G16" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="I16" s="19">
         <f>SUM(J16:K16)</f>
@@ -3606,7 +3526,7 @@
       </c>
       <c r="L16" s="21"/>
       <c r="M16" s="6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="N16" s="22">
         <f>C16</f>
@@ -3615,6 +3535,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
@@ -3631,21 +3566,6 @@
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3653,21 +3573,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3811,24 +3716,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741A764F-DFF5-4AE4-B0E7-77BD148FABB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3844,4 +3747,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>